<commit_message>
Desafío: Catálogo con MAPS y Promises
</commit_message>
<xml_diff>
--- a/public/data/productos.xlsx
+++ b/public/data/productos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmanc\Documents\Personal\Coder House\React\Proyecto Final\proyecto-final-react\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Proyectos\React\proyecto-final-react\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70D72CB-9CAD-4769-91EC-E993C1AA816C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A8617993-1235-4001-B542-120A82400DF9}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="productos" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -219,9 +218,6 @@
     <t>Proyector</t>
   </si>
   <si>
-    <t>Tortuga 12w ovalada blanca, medidas 20,0 x 9,8 x 4,5 cm luz cálida</t>
-  </si>
-  <si>
     <t>Proyector 10w 6000K</t>
   </si>
   <si>
@@ -267,9 +263,6 @@
     <t>imagen</t>
   </si>
   <si>
-    <t>Tortuga 18w ovalada blanca, medidas 23,0 x 10,5 x 2,5 cm luz cálida</t>
-  </si>
-  <si>
     <t>Lámpara Gota</t>
   </si>
   <si>
@@ -367,12 +360,18 @@
   </si>
   <si>
     <t>tortuga_4507.jpg</t>
+  </si>
+  <si>
+    <t>Tortuga 12w ovalada blanca, 20,0 x 9,8 x 4,5 cm luz cálida</t>
+  </si>
+  <si>
+    <t>Tortuga 18w ovalada blanca, 23,0 x 10,5 x 2,5 cm luz cálida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -766,58 +765,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68718C7-0E07-42FB-A69D-24E0FA5539C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" customWidth="1"/>
-    <col min="3" max="3" width="35.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="45.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3120</v>
       </c>
@@ -838,10 +837,10 @@
         <v>67.52</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3121</v>
       </c>
@@ -855,7 +854,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -864,10 +863,10 @@
         <v>67.52</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3122</v>
       </c>
@@ -887,10 +886,10 @@
         <v>72.209999999999994</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3123</v>
       </c>
@@ -904,7 +903,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>20</v>
@@ -913,10 +912,10 @@
         <v>72.209999999999994</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3124</v>
       </c>
@@ -936,10 +935,10 @@
         <v>75.02</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3125</v>
       </c>
@@ -959,10 +958,10 @@
         <v>75.02</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3126</v>
       </c>
@@ -982,10 +981,10 @@
         <v>77.45</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3127</v>
       </c>
@@ -1005,10 +1004,10 @@
         <v>77.45</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3133</v>
       </c>
@@ -1028,14 +1027,14 @@
         <v>79.989999999999995</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1043</v>
       </c>
@@ -1055,10 +1054,10 @@
         <v>103.15</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1053</v>
       </c>
@@ -1078,10 +1077,10 @@
         <v>116.52</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1101,14 +1100,14 @@
         <v>103.15</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3029</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -1131,19 +1130,19 @@
         <v>467</v>
       </c>
       <c r="H17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3260</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
@@ -1158,14 +1157,14 @@
         <v>97.53</v>
       </c>
       <c r="H19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3424</v>
       </c>
@@ -1185,14 +1184,14 @@
         <v>163.16</v>
       </c>
       <c r="H21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3611</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -1215,10 +1214,10 @@
         <v>243.82</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3613</v>
       </c>
@@ -1238,10 +1237,10 @@
         <v>376.53</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>3615</v>
       </c>
@@ -1261,14 +1260,14 @@
         <v>517.64</v>
       </c>
       <c r="H25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>4503</v>
       </c>
@@ -1279,10 +1278,10 @@
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27">
         <v>5</v>
@@ -1291,10 +1290,10 @@
         <v>693.78</v>
       </c>
       <c r="H27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4507</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -1314,19 +1313,19 @@
         <v>882.67</v>
       </c>
       <c r="H28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>5703</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -1341,15 +1340,15 @@
         <v>518.36</v>
       </c>
       <c r="H30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>5705</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -1364,15 +1363,15 @@
         <v>518.36</v>
       </c>
       <c r="H31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>5808</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -1387,15 +1386,15 @@
         <v>817.46</v>
       </c>
       <c r="H32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>5852</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -1404,7 +1403,7 @@
         <v>52</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -1413,15 +1412,15 @@
         <v>492.49</v>
       </c>
       <c r="H33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>5856</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -1436,15 +1435,15 @@
         <v>817.46</v>
       </c>
       <c r="H34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>5858</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1459,15 +1458,15 @@
         <v>817.46</v>
       </c>
       <c r="H35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>5861</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1482,14 +1481,14 @@
         <v>1246.99</v>
       </c>
       <c r="H36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>7603</v>
       </c>
@@ -1497,13 +1496,13 @@
         <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
         <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F38">
         <v>5</v>
@@ -1512,14 +1511,14 @@
         <v>492.49</v>
       </c>
       <c r="H38" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2501</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -1539,10 +1538,10 @@
         <v>1341.44</v>
       </c>
       <c r="H40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2503</v>
       </c>
@@ -1553,7 +1552,7 @@
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -1562,21 +1561,21 @@
         <v>2372.54</v>
       </c>
       <c r="H41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primera Entrega del Proyecto Final
</commit_message>
<xml_diff>
--- a/public/data/productos.xlsx
+++ b/public/data/productos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Proyectos\React\proyecto-final-react\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmanc\Documents\Personal\Coder House\React\Proyecto Final\proyecto-final-react\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8326D9-B48E-4C2F-B89B-01D09BECFA2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10560"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="productos" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
   <si>
     <t>Lámpara Dicroica 5w 38° 3000K</t>
   </si>
@@ -50,24 +51,6 @@
     <t>Lámpara Dicroica 5w 38° Blister 6000K</t>
   </si>
   <si>
-    <t>Lámpara Bulbo</t>
-  </si>
-  <si>
-    <t>Lámpara Dicrocia</t>
-  </si>
-  <si>
-    <t>Luminaria emergencia</t>
-  </si>
-  <si>
-    <t>Lámpara Globo</t>
-  </si>
-  <si>
-    <t>Lámpara Perfume</t>
-  </si>
-  <si>
-    <t>Lámpara Serie T</t>
-  </si>
-  <si>
     <t>Lámpara Dicroica 7w 38° 3000K</t>
   </si>
   <si>
@@ -212,9 +195,6 @@
     <t>Lámpara Bulbo 15w luz fría equivalente a 120w lámpara común</t>
   </si>
   <si>
-    <t>Tortuga</t>
-  </si>
-  <si>
     <t>Proyector</t>
   </si>
   <si>
@@ -263,15 +243,6 @@
     <t>imagen</t>
   </si>
   <si>
-    <t>Lámpara Gota</t>
-  </si>
-  <si>
-    <t>Luminaria embutir</t>
-  </si>
-  <si>
-    <t>Luminaria aplicar</t>
-  </si>
-  <si>
     <t>bulbo_3120.jpg</t>
   </si>
   <si>
@@ -366,12 +337,54 @@
   </si>
   <si>
     <t>Tortuga 18w ovalada blanca, 23,0 x 10,5 x 2,5 cm luz cálida</t>
+  </si>
+  <si>
+    <t>subtipo</t>
+  </si>
+  <si>
+    <t>Luminaria</t>
+  </si>
+  <si>
+    <t>lampara</t>
+  </si>
+  <si>
+    <t>bulbo</t>
+  </si>
+  <si>
+    <t>dicroica</t>
+  </si>
+  <si>
+    <t>globo</t>
+  </si>
+  <si>
+    <t>gota</t>
+  </si>
+  <si>
+    <t>perfume</t>
+  </si>
+  <si>
+    <t>serieT</t>
+  </si>
+  <si>
+    <t>tortuga</t>
+  </si>
+  <si>
+    <t>embutir</t>
+  </si>
+  <si>
+    <t>aplicar</t>
+  </si>
+  <si>
+    <t>proyector</t>
+  </si>
+  <si>
+    <t>emergencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -434,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -451,6 +464,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -765,817 +779,922 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="45.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="35.54296875" customWidth="1"/>
+    <col min="5" max="5" width="59" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3120</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3">
+      <c r="B3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>67.52</v>
       </c>
-      <c r="H3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4">
         <v>20</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>67.52</v>
       </c>
-      <c r="H4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3122</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>72.209999999999994</v>
       </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3123</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
+        <v>106</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6">
         <v>20</v>
       </c>
-      <c r="G6" s="7">
+      <c r="H6" s="7">
         <v>72.209999999999994</v>
       </c>
-      <c r="H6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3124</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
+        <v>106</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7">
         <v>20</v>
       </c>
-      <c r="G7" s="7">
+      <c r="H7" s="7">
         <v>75.02</v>
       </c>
-      <c r="H7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
+        <v>106</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
         <v>40</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="7">
         <v>75.02</v>
       </c>
-      <c r="H8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3126</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
+        <v>106</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
         <v>20</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="7">
         <v>77.45</v>
       </c>
-      <c r="H9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3127</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
+        <v>106</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10">
         <v>20</v>
       </c>
-      <c r="G10" s="7">
+      <c r="H10" s="7">
         <v>77.45</v>
       </c>
-      <c r="H10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3133</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
+        <v>106</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11">
         <v>20</v>
       </c>
-      <c r="G11" s="7">
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11" s="7">
         <v>79.989999999999995</v>
       </c>
-      <c r="H11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1043</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
         <v>0</v>
       </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13">
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13">
         <v>10</v>
       </c>
-      <c r="G13" s="7">
+      <c r="H13" s="7">
         <v>103.15</v>
       </c>
-      <c r="H13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1053</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
+      <c r="B14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14">
         <v>10</v>
       </c>
-      <c r="G14" s="7">
+      <c r="H14" s="7">
         <v>116.52</v>
       </c>
-      <c r="H14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15">
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
         <v>10</v>
       </c>
-      <c r="G15" s="7">
+      <c r="H15" s="7">
         <v>103.15</v>
       </c>
-      <c r="H15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>3029</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
       <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17">
         <v>5</v>
       </c>
-      <c r="G17" s="7">
+      <c r="H17" s="7">
         <v>467</v>
       </c>
-      <c r="H17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>3260</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" t="s">
-        <v>27</v>
+        <v>106</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19">
         <v>10</v>
       </c>
-      <c r="G19" s="7">
+      <c r="H19" s="7">
         <v>97.53</v>
       </c>
-      <c r="H19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>3424</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
+      <c r="B21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21">
         <v>5</v>
       </c>
-      <c r="G21" s="7">
+      <c r="H21" s="7">
         <v>163.16</v>
       </c>
-      <c r="H21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>3611</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
+      <c r="B23" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23">
         <v>10</v>
       </c>
-      <c r="G23" s="7">
+      <c r="H23" s="7">
         <v>243.82</v>
       </c>
-      <c r="H23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3613</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
+      <c r="B24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24">
         <v>10</v>
       </c>
-      <c r="G24" s="7">
+      <c r="H24" s="7">
         <v>376.53</v>
       </c>
-      <c r="H24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3615</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
+      <c r="B25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25">
         <v>10</v>
       </c>
-      <c r="G25" s="7">
+      <c r="H25" s="7">
         <v>517.64</v>
       </c>
-      <c r="H25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>4503</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>35</v>
+        <v>105</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27">
         <v>5</v>
       </c>
-      <c r="G27" s="7">
+      <c r="H27" s="7">
         <v>693.78</v>
       </c>
-      <c r="H27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>4507</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28">
         <v>5</v>
       </c>
-      <c r="G28" s="7">
+      <c r="H28" s="7">
         <v>882.67</v>
       </c>
-      <c r="H28" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>5703</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" t="s">
-        <v>15</v>
+        <v>105</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30">
         <v>5</v>
       </c>
-      <c r="G30" s="7">
+      <c r="H30" s="7">
         <v>518.36</v>
       </c>
-      <c r="H30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>5705</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31">
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31">
         <v>5</v>
       </c>
-      <c r="G31" s="7">
+      <c r="H31" s="7">
         <v>518.36</v>
       </c>
-      <c r="H31" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>5808</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
+        <v>105</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32">
         <v>5</v>
       </c>
-      <c r="G32" s="7">
+      <c r="H32" s="7">
         <v>817.46</v>
       </c>
-      <c r="H32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>5852</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" t="s">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
-        <v>52</v>
-      </c>
       <c r="E33" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33">
         <v>5</v>
       </c>
-      <c r="G33" s="7">
+      <c r="H33" s="7">
         <v>492.49</v>
       </c>
-      <c r="H33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>5856</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" t="s">
-        <v>16</v>
+        <v>105</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34">
         <v>5</v>
       </c>
-      <c r="G34" s="7">
+      <c r="H34" s="7">
         <v>817.46</v>
       </c>
-      <c r="H34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>5858</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35">
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35">
         <v>5</v>
       </c>
-      <c r="G35" s="7">
+      <c r="H35" s="7">
         <v>817.46</v>
       </c>
-      <c r="H35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>5861</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="s">
         <v>5</v>
       </c>
-      <c r="D36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36">
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36">
         <v>5</v>
       </c>
-      <c r="G36" s="7">
+      <c r="H36" s="7">
         <v>1246.99</v>
       </c>
-      <c r="H36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>7603</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38">
+        <v>48</v>
+      </c>
+      <c r="F38" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38">
         <v>5</v>
       </c>
-      <c r="G38" s="7">
+      <c r="H38" s="7">
         <v>492.49</v>
       </c>
-      <c r="H38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2501</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>29</v>
+        <v>105</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40">
+        <v>23</v>
+      </c>
+      <c r="E40" t="s">
+        <v>58</v>
+      </c>
+      <c r="G40">
         <v>2</v>
       </c>
-      <c r="G40" s="7">
+      <c r="H40" s="7">
         <v>1341.44</v>
       </c>
-      <c r="H40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2503</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
+        <v>105</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41">
         <v>2</v>
       </c>
-      <c r="G41" s="7">
+      <c r="H41" s="7">
         <v>2372.54</v>
       </c>
-      <c r="H41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Desafío Clase 12 - Firestore Item Collection Se modifico ItemListContainer e ItemDetailContainer para acceder a bbdd en Firebase Las imagenes se cargaron con url que apunta a carpeta compartida de Google Drive
</commit_message>
<xml_diff>
--- a/public/data/productos.xlsx
+++ b/public/data/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmanc\Documents\Personal\Coder House\React\Proyecto Final\proyecto-final-react\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8326D9-B48E-4C2F-B89B-01D09BECFA2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A13BE73-C8FE-47E0-A16D-EC6EC45D4627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="152">
   <si>
     <t>Lámpara Dicroica 5w 38° 3000K</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Lámpara Bulbo 15w luz fría equivalente a 120w lámpara común</t>
   </si>
   <si>
-    <t>Proyector</t>
-  </si>
-  <si>
     <t>Proyector 10w 6000K</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>subtipo</t>
   </si>
   <si>
-    <t>Luminaria</t>
-  </si>
-  <si>
     <t>lampara</t>
   </si>
   <si>
@@ -379,6 +373,114 @@
   </si>
   <si>
     <t>emergencia</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1pDWVGAXL9BxmlpMWMcEqgRHKO5P7WKkz/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ECFxqV1GDoTEtW1pSchECRxM4aHos2iD/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1lZ5psGJcB8GbrV6xLG2MlF3Da7CCFUnm/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13mY7MofLILW89nauI3dG9_YYSxdfT7ZB/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15FQW8eFG-r3-yFbsxKHg4lgajYnKyIPU/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15gSS4k_iGCz0E5T76DeZHbCAfnDgPwYS/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15txa-3znTyJ-Cgsn8qWAdnys_mdMWQf0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1AIn7pkcXNgijnsnGZji_oLy3CpqJfR-R/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1AaIuKwtK--86vxEvAhZEcWweOBMdYfHP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1EHUYdl97L04hblp3FNit1W5jOyRdiNyu/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1EudRNcWZViCnr_wM1gsW3vEeJ7MddEtM/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1FViy-ZaDahq-4Ori9sxw6ykSePe82WRv/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1G7xjTdYYsgX-e9Vbk7pTECgjegNkgNQg/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1LjaGr8N_Vx7Mhzl_dWr0ViJXg5CWxmvY/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RpzH09hKe-W1myQcJ7eHwIIc0yhEno1h/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1U7myk6i8stzV1oh17LPf9ub938UYM0QK/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1UhyGJSmpkPExV7ePQk51y0PTWboLagxr/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1eTFr1G9PvlCvCohZPkD1LT7biaNDTKRI/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1hMPujSSFsFyUUXdxyrU2rF-RYVb2GqQC/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1li296pBsQKeOnAQ5VJmUfq4TxdYVpm-E/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1m9jpyrqxwTY9lcvmRzG2O5KNzkHbXC5-/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1pOy6YJruekztZYYRz1bkJdWJe420uv4o/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1qQggQrE0fQf9r8iKLBRdhm5wuRCIxxVw/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ssU3n6Ypx4DGTznbVm_JHENIY6cqWHJ4/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1t9FSIRjyK-YWE79ellHv3GnD91SNkmQQ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1wNPZabtGcXhu2uWIjQrihcIIqvFxOxy8/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1whOlXXUtBxUXlXCwyvoouXg_e68Dfni4/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1xHhLRV5rdxvnYnD-C58hZPdrmgfdD9e3/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1z6UX1-xAtvNUaAq3UeN8_RiggYUnY1S6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1zTncj2OVoL9r_uF0MleirNk-MoFVGKye/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1zoILv7wNI8TylVHjECyG3VbhOBYVKBW0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Lámpara Bulbo 15w luz cálida equivalente a 120w lámpara común</t>
+  </si>
+  <si>
+    <t>Lámpara Bulbo 15w 3000K</t>
+  </si>
+  <si>
+    <t>bulbo_3132.jpg</t>
+  </si>
+  <si>
+    <t>luminaria</t>
   </si>
 </sst>
 </file>
@@ -388,7 +490,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +521,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -443,11 +553,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -465,8 +576,10 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -780,13 +893,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,50 +912,54 @@
     <col min="6" max="6" width="13.7265625" customWidth="1"/>
     <col min="7" max="7" width="11.453125" customWidth="1"/>
     <col min="8" max="8" width="15.453125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="45.453125" customWidth="1"/>
+    <col min="9" max="9" width="27.54296875" customWidth="1"/>
+    <col min="10" max="10" width="82.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3120</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -858,18 +975,21 @@
         <v>67.52</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -878,7 +998,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -887,18 +1007,21 @@
         <v>67.52</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3122</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -913,18 +1036,21 @@
         <v>72.209999999999994</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3123</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -933,7 +1059,7 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -942,23 +1068,26 @@
         <v>72.209999999999994</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3124</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G7">
@@ -968,18 +1097,21 @@
         <v>75.02</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -994,18 +1126,21 @@
         <v>75.02</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="J8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3126</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -1020,18 +1155,21 @@
         <v>77.45</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="J9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3127</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -1046,24 +1184,27 @@
         <v>77.45</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="J10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>3133</v>
+        <v>3132</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="G11">
         <v>20</v>
@@ -1072,380 +1213,419 @@
         <v>79.989999999999995</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+        <v>150</v>
+      </c>
+      <c r="J11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>3133</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12" s="7">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>1043</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>36</v>
-      </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-      <c r="H13" s="7">
-        <v>103.15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>1053</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
       </c>
       <c r="G14">
         <v>10</v>
       </c>
       <c r="H14" s="7">
-        <v>116.52</v>
+        <v>103.15</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>80</v>
+      </c>
+      <c r="J14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>1053</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G15">
         <v>10</v>
       </c>
       <c r="H15" s="7">
+        <v>116.52</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16" s="7">
         <v>103.15</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>3029</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>467</v>
+      </c>
+      <c r="I18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>3029</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="J18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>3260</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20" s="7">
+        <v>97.53</v>
+      </c>
+      <c r="I20" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>3424</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17">
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22">
         <v>5</v>
       </c>
-      <c r="H17" s="7">
-        <v>467</v>
-      </c>
-      <c r="I17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>3260</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="H22" s="7">
+        <v>163.16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>3611</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="H19" s="7">
-        <v>97.53</v>
-      </c>
-      <c r="I19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>3424</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21">
-        <v>5</v>
-      </c>
-      <c r="H21" s="7">
-        <v>163.16</v>
-      </c>
-      <c r="I21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>3611</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>43</v>
       </c>
-      <c r="F23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23" s="7">
-        <v>243.82</v>
-      </c>
-      <c r="I23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>3613</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" t="s">
-        <v>44</v>
+      <c r="F24" t="s">
+        <v>59</v>
       </c>
       <c r="G24">
         <v>10</v>
       </c>
       <c r="H24" s="7">
-        <v>376.53</v>
+        <v>243.82</v>
       </c>
       <c r="I24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="J24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>3615</v>
+        <v>3613</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25">
         <v>10</v>
       </c>
       <c r="H25" s="7">
+        <v>376.53</v>
+      </c>
+      <c r="I25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>3615</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="H26" s="7">
         <v>517.64</v>
       </c>
-      <c r="I25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="I26" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
         <v>4503</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B28" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
         <v>29</v>
       </c>
-      <c r="E27" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27">
-        <v>5</v>
-      </c>
-      <c r="H27" s="7">
-        <v>693.78</v>
-      </c>
-      <c r="I27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>4507</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="F28" t="s">
+        <v>62</v>
       </c>
       <c r="G28">
         <v>5</v>
       </c>
       <c r="H28" s="7">
+        <v>693.78</v>
+      </c>
+      <c r="I28" t="s">
+        <v>99</v>
+      </c>
+      <c r="J28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>4507</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29" s="7">
         <v>882.67</v>
       </c>
-      <c r="I28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+      <c r="I29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
         <v>5703</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B31" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" t="s">
         <v>9</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>33</v>
-      </c>
-      <c r="G30">
-        <v>5</v>
-      </c>
-      <c r="H30" s="7">
-        <v>518.36</v>
-      </c>
-      <c r="I30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>5705</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>31</v>
       </c>
       <c r="G31">
         <v>5</v>
@@ -1454,105 +1634,117 @@
         <v>518.36</v>
       </c>
       <c r="I31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="J31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>5808</v>
+        <v>5705</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G32">
         <v>5</v>
       </c>
       <c r="H32" s="7">
-        <v>817.46</v>
+        <v>518.36</v>
       </c>
       <c r="I32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="J32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>5852</v>
+        <v>5808</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="G33">
         <v>5</v>
       </c>
       <c r="H33" s="7">
-        <v>492.49</v>
+        <v>817.46</v>
       </c>
       <c r="I33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+      <c r="J33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>5856</v>
+        <v>5852</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>62</v>
       </c>
       <c r="G34">
         <v>5</v>
       </c>
       <c r="H34" s="7">
-        <v>817.46</v>
+        <v>492.49</v>
       </c>
       <c r="I34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="J34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>5858</v>
+        <v>5856</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G35">
         <v>5</v>
@@ -1561,144 +1753,192 @@
         <v>817.46</v>
       </c>
       <c r="I35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="J35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>5861</v>
+        <v>5858</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="G36">
         <v>5</v>
       </c>
       <c r="H36" s="7">
+        <v>817.46</v>
+      </c>
+      <c r="I36" t="s">
+        <v>94</v>
+      </c>
+      <c r="J36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>5861</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37" s="7">
         <v>1246.99</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
+        <v>95</v>
+      </c>
+      <c r="J37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>7603</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39" s="7">
+        <v>492.49</v>
+      </c>
+      <c r="I39" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>7603</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="J39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>2501</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" t="s">
         <v>57</v>
-      </c>
-      <c r="E38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" t="s">
-        <v>62</v>
-      </c>
-      <c r="G38">
-        <v>5</v>
-      </c>
-      <c r="H38" s="7">
-        <v>492.49</v>
-      </c>
-      <c r="I38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
-        <v>2501</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D40" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" t="s">
-        <v>58</v>
-      </c>
-      <c r="G40">
-        <v>2</v>
-      </c>
-      <c r="H40" s="7">
-        <v>1341.44</v>
-      </c>
-      <c r="I40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>2503</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" t="s">
-        <v>59</v>
       </c>
       <c r="G41">
         <v>2</v>
       </c>
       <c r="H41" s="7">
+        <v>1341.44</v>
+      </c>
+      <c r="I41" t="s">
+        <v>97</v>
+      </c>
+      <c r="J41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>2503</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42" s="7">
         <v>2372.54</v>
       </c>
-      <c r="I41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I42" t="s">
+        <v>98</v>
+      </c>
+      <c r="J42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
     </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{072C9FA6-3E42-42CF-BC6A-F17EEBE8EE14}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{6DEDC503-4BCB-4E42-88E5-AB2D3631B4DB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>